<commit_message>
added receipt and remarks
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453E1A54-6ACB-4E7F-90B0-27DE2538DDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FBD540-250C-4DA7-8F04-DA1836D2C1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="270" windowWidth="21600" windowHeight="14190" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance_01-Apr-2025_Onwards" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="232">
   <si>
     <t xml:space="preserve">S.no </t>
   </si>
@@ -800,6 +800,9 @@
   </si>
   <si>
     <t>by amit</t>
+  </si>
+  <si>
+    <t>sandeep</t>
   </si>
 </sst>
 </file>
@@ -9405,7 +9408,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9472,6 +9475,9 @@
       <c r="F3">
         <v>182204</v>
       </c>
+      <c r="G3" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D4" s="62">
@@ -9496,6 +9502,9 @@
       </c>
       <c r="F5">
         <v>29811</v>
+      </c>
+      <c r="G5" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
g21 g33 122 122a maint
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA11908-25EE-4B7E-A0F9-AC1A1987F0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03966E8-5349-4E1A-A81A-A81E653FEB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
@@ -741,10 +741,6 @@
     <t>Total EB Collection from 08-Apr-2025</t>
   </si>
   <si>
-    <t xml:space="preserve">Confident Group
-</t>
-  </si>
-  <si>
     <t>With Sandeep</t>
   </si>
   <si>
@@ -816,6 +812,10 @@
   </si>
   <si>
     <t xml:space="preserve">maint. chunk handed over to residential </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayur
+</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1157,6 +1157,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1498,9 +1501,9 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
+      <selection pane="bottomLeft" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,7 +2383,9 @@
         <f t="shared" si="0"/>
         <v>7770</v>
       </c>
-      <c r="K24" s="21"/>
+      <c r="K24" s="21">
+        <v>7770</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -2851,7 +2856,9 @@
         <f t="shared" si="0"/>
         <v>6077</v>
       </c>
-      <c r="K37" s="21"/>
+      <c r="K37" s="21">
+        <v>6077</v>
+      </c>
     </row>
     <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
@@ -3800,7 +3807,7 @@
         <v>69</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E64" s="15">
         <v>694</v>
@@ -3966,7 +3973,9 @@
         <f t="shared" si="2"/>
         <v>7459</v>
       </c>
-      <c r="K68" s="21"/>
+      <c r="K68" s="21">
+        <v>7459</v>
+      </c>
     </row>
     <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
@@ -3975,8 +3984,8 @@
       <c r="B69" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C69" s="37" t="s">
-        <v>211</v>
+      <c r="C69" s="69" t="s">
+        <v>235</v>
       </c>
       <c r="D69" s="34"/>
       <c r="E69" s="34">
@@ -3999,7 +4008,9 @@
         <f t="shared" si="2"/>
         <v>3641</v>
       </c>
-      <c r="K69" s="21"/>
+      <c r="K69" s="21">
+        <v>3641</v>
+      </c>
     </row>
     <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
@@ -4156,7 +4167,7 @@
       </c>
       <c r="K74">
         <f>SUM(K2:K73)</f>
-        <v>248416</v>
+        <v>273363</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -4199,8 +4210,8 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U73" sqref="U73"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9425,7 +9436,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9460,7 +9471,7 @@
       </c>
       <c r="C2" s="3">
         <f>'Maintenance_01-Apr-2025_Onwards'!K74</f>
-        <v>248416</v>
+        <v>273363</v>
       </c>
       <c r="D2" s="62">
         <v>45686</v>
@@ -9472,7 +9483,7 @@
         <v>18043</v>
       </c>
       <c r="G2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -9487,13 +9498,13 @@
         <v>45706</v>
       </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F3">
         <v>182204</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -9501,13 +9512,13 @@
         <v>45733</v>
       </c>
       <c r="E4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F4">
         <v>182412</v>
       </c>
       <c r="G4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -9521,7 +9532,7 @@
         <v>29811</v>
       </c>
       <c r="G5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -9535,7 +9546,7 @@
         <v>3630</v>
       </c>
       <c r="G6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -9544,7 +9555,7 @@
       </c>
       <c r="C7" s="3">
         <f>SUM(C1:C6)</f>
-        <v>1019846</v>
+        <v>1044793</v>
       </c>
       <c r="D7" s="62">
         <v>45757</v>
@@ -9557,7 +9568,7 @@
         <v>6082</v>
       </c>
       <c r="G7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -9565,13 +9576,13 @@
         <v>45761</v>
       </c>
       <c r="E8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F8">
         <v>245778</v>
       </c>
       <c r="G8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -9586,13 +9597,13 @@
         <v>45761</v>
       </c>
       <c r="E9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F9">
         <v>32745</v>
       </c>
       <c r="G9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -9600,19 +9611,19 @@
         <v>174</v>
       </c>
       <c r="C10" s="3">
-        <v>80651</v>
+        <v>91651</v>
       </c>
       <c r="D10" s="62">
         <v>45761</v>
       </c>
       <c r="E10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F10">
         <v>142355</v>
       </c>
       <c r="G10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -9620,7 +9631,7 @@
         <v>175</v>
       </c>
       <c r="C11" s="3">
-        <v>3821</v>
+        <v>17668</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -9633,7 +9644,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" s="3">
         <f>withWhom!H26</f>
@@ -9649,7 +9660,7 @@
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>177298</v>
+        <v>202145</v>
       </c>
       <c r="E15" t="s">
         <v>172</v>
@@ -9668,7 +9679,7 @@
       </c>
       <c r="C17" s="3">
         <f>C7-F15</f>
-        <v>176786</v>
+        <v>201733</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -9687,7 +9698,7 @@
       </c>
       <c r="C20" s="3">
         <f>C17-C15</f>
-        <v>-512</v>
+        <v>-412</v>
       </c>
       <c r="E20" s="38"/>
     </row>
@@ -13638,7 +13649,7 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B3" s="66"/>
       <c r="C3" s="66"/>
@@ -13647,31 +13658,31 @@
       </c>
       <c r="E3" s="66"/>
       <c r="F3" s="66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G3" s="66"/>
       <c r="H3" s="67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I3" s="66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B4" s="11">
         <v>117636</v>
       </c>
       <c r="C4" s="68" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" s="11">
         <v>67347</v>
       </c>
       <c r="E4" s="68" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F4" s="11">
         <v>40543</v>
@@ -13682,7 +13693,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5" s="11">
         <v>9984</v>
@@ -13722,7 +13733,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7" s="11">
         <v>5299</v>
@@ -13748,7 +13759,7 @@
         <v>14500</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D8" s="11">
         <v>13912</v>
@@ -13768,7 +13779,7 @@
         <v>8550</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D9" s="11">
         <v>13916</v>
@@ -13802,7 +13813,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="11">
         <v>11079</v>
@@ -13862,7 +13873,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="11">
         <v>8100</v>
@@ -13890,7 +13901,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B16" s="11">
         <v>-53000</v>
@@ -13926,7 +13937,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C20" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
g37 m and e paid
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03966E8-5349-4E1A-A81A-A81E653FEB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0B5279-5E72-4DAD-AE50-EA0E1F25EBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance_01-Apr-2025_Onwards" sheetId="9" r:id="rId1"/>
@@ -1500,10 +1500,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E3C748-2165-4E26-87D0-2D40C997FFD8}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="M37" sqref="M37"/>
+      <selection pane="bottomLeft" activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3002,7 +3002,9 @@
         <f t="shared" si="0"/>
         <v>3455</v>
       </c>
-      <c r="K41" s="21"/>
+      <c r="K41" s="21">
+        <v>3455</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
@@ -4167,7 +4169,7 @@
       </c>
       <c r="K74">
         <f>SUM(K2:K73)</f>
-        <v>273363</v>
+        <v>276818</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -4210,8 +4212,8 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V40" sqref="V40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7120,7 +7122,9 @@
         <f t="shared" si="18"/>
         <v>760</v>
       </c>
-      <c r="U41" s="21"/>
+      <c r="U41" s="21">
+        <v>760</v>
+      </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="45">
@@ -9357,7 +9361,7 @@
       <c r="T73" s="21"/>
       <c r="U73" s="20">
         <f>SUM(U2:U72)</f>
-        <v>129012</v>
+        <v>129772</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -9435,8 +9439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C901BC-37D1-4CF5-9271-04B7C9971E6A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9471,7 +9475,7 @@
       </c>
       <c r="C2" s="3">
         <f>'Maintenance_01-Apr-2025_Onwards'!K74</f>
-        <v>273363</v>
+        <v>276818</v>
       </c>
       <c r="D2" s="62">
         <v>45686</v>
@@ -9492,7 +9496,7 @@
       </c>
       <c r="C3" s="3">
         <f>EB!U73</f>
-        <v>129012</v>
+        <v>129772</v>
       </c>
       <c r="D3" s="62">
         <v>45706</v>
@@ -9555,7 +9559,7 @@
       </c>
       <c r="C7" s="3">
         <f>SUM(C1:C6)</f>
-        <v>1044793</v>
+        <v>1049008</v>
       </c>
       <c r="D7" s="62">
         <v>45757</v>
@@ -9639,7 +9643,8 @@
         <v>179</v>
       </c>
       <c r="C12" s="3">
-        <v>92538</v>
+        <f>92538+4215</f>
+        <v>96753</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -9660,7 +9665,7 @@
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>202145</v>
+        <v>206360</v>
       </c>
       <c r="E15" t="s">
         <v>172</v>
@@ -9679,7 +9684,7 @@
       </c>
       <c r="C17" s="3">
         <f>C7-F15</f>
-        <v>201733</v>
+        <v>205948</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
april diesel expense added
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E44680-DF2E-4200-AD96-DC21F9E738EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2631431-D57A-4FF8-A09C-D469DEEDD4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance_01-Apr-2025_Onwards" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="237">
   <si>
     <t xml:space="preserve">S.no </t>
   </si>
@@ -1503,10 +1503,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E3C748-2165-4E26-87D0-2D40C997FFD8}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4219,8 +4219,8 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V15" sqref="V15"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U67" sqref="U67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9448,7 +9448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C901BC-37D1-4CF5-9271-04B7C9971E6A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -9624,8 +9624,8 @@
         <v>174</v>
       </c>
       <c r="C10" s="3">
-        <f>91651+6687-10000+2700</f>
-        <v>91038</v>
+        <f>91651+6687-10000+2700-36400</f>
+        <v>54638</v>
       </c>
       <c r="D10" s="62">
         <v>45761</v>
@@ -9648,6 +9648,9 @@
         <f>17668+2566</f>
         <v>20234</v>
       </c>
+      <c r="D11" s="62">
+        <v>45763</v>
+      </c>
       <c r="E11" t="s">
         <v>236</v>
       </c>
@@ -9666,6 +9669,18 @@
         <f>92538+4215</f>
         <v>96753</v>
       </c>
+      <c r="D12" s="62">
+        <v>45756</v>
+      </c>
+      <c r="E12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12">
+        <v>18198</v>
+      </c>
+      <c r="G12" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -9675,6 +9690,18 @@
         <f>withWhom!H26</f>
         <v>0</v>
       </c>
+      <c r="D13" s="62">
+        <v>45763</v>
+      </c>
+      <c r="E13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13">
+        <v>18198</v>
+      </c>
+      <c r="G13" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
@@ -9685,14 +9712,14 @@
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>208313</v>
+        <v>171913</v>
       </c>
       <c r="E15" t="s">
         <v>172</v>
       </c>
       <c r="F15">
         <f>SUM(F2:F14)</f>
-        <v>853060</v>
+        <v>889456</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -9704,7 +9731,7 @@
       </c>
       <c r="C17" s="3">
         <f>C7-F15</f>
-        <v>207901</v>
+        <v>171505</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -9723,7 +9750,7 @@
       </c>
       <c r="C20" s="3">
         <f>C17-C15</f>
-        <v>-412</v>
+        <v>-408</v>
       </c>
       <c r="E20" s="38"/>
     </row>

</xml_diff>

<commit_message>
124 m and eb recorded
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2631431-D57A-4FF8-A09C-D469DEEDD4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7358DEF-F900-4463-8BBA-5EFE280729F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance_01-Apr-2025_Onwards" sheetId="9" r:id="rId1"/>
@@ -1504,27 +1504,27 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
+      <selection pane="bottomLeft" activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="54" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="54" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="54" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="54" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="54" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="54" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="54" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="54" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="54" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="54" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>6414</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>6687</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>26599</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="K6" s="21"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1812,7 +1812,7 @@
       </c>
       <c r="K8" s="21"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="K10" s="21"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>5163</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>3010</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>3637</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>4086</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>3264</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>10650</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>2522</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>3146</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>7770</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>3691</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>4203</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>7297</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>4710</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>7044</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>21982</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>14858</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>6077</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>13087</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="K40" s="21"/>
     </row>
-    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>3455</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>4240</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>24798</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="K45" s="21"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="K46" s="21"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -3231,7 +3231,7 @@
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -3266,7 +3266,7 @@
       </c>
       <c r="K48" s="21"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="K49" s="21"/>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>3242</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -3373,7 +3373,7 @@
       </c>
       <c r="K51" s="21"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>7836</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>4576</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="K54" s="21"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>3614</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="K56" s="21"/>
     </row>
-    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>10113</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -3626,7 +3626,7 @@
       </c>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>3382</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="K61" s="21"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -3770,7 +3770,7 @@
       </c>
       <c r="K62" s="21"/>
     </row>
-    <row r="63" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="K63" s="21"/>
     </row>
-    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>3151</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>11827</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="K67" s="21"/>
     </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>7459</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>3641</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="K70" s="21"/>
     </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -4089,9 +4089,11 @@
         <f t="shared" si="2"/>
         <v>2629</v>
       </c>
-      <c r="K71" s="21"/>
-    </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K71" s="21">
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -4126,7 +4128,7 @@
       </c>
       <c r="K72" s="21"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -4163,7 +4165,7 @@
         <v>10666</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E74" s="2">
         <f>SUM(E2:E73)</f>
         <v>57993</v>
@@ -4176,35 +4178,35 @@
       </c>
       <c r="K74">
         <f>SUM(K2:K73)</f>
-        <v>286205</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+        <v>288834</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C77"/>
       <c r="E77" s="54"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C78" s="2"/>
     </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D84"/>
       <c r="E84" s="54"/>
       <c r="F84" s="57"/>
     </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D85"/>
       <c r="E85" s="54"/>
     </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D86" s="38"/>
       <c r="E86" s="54"/>
       <c r="F86" s="57"/>
     </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D87"/>
       <c r="E87" s="54"/>
     </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D88"/>
       <c r="E88" s="54"/>
     </row>
@@ -4219,16 +4221,16 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U67" sqref="U67"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>147</v>
       </c>
@@ -4293,7 +4295,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>2</v>
       </c>
@@ -4366,7 +4368,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
@@ -4435,7 +4437,7 @@
       </c>
       <c r="U3" s="21"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
@@ -4505,7 +4507,7 @@
         <v>2551</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>5</v>
       </c>
@@ -4578,7 +4580,7 @@
         <v>8354</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
@@ -4649,7 +4651,7 @@
       </c>
       <c r="U6" s="21"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
@@ -4718,7 +4720,7 @@
       </c>
       <c r="U7" s="21"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
@@ -4787,7 +4789,7 @@
       </c>
       <c r="U8" s="21"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>9</v>
       </c>
@@ -4856,7 +4858,7 @@
       </c>
       <c r="U9" s="21"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>10</v>
       </c>
@@ -4925,7 +4927,7 @@
       </c>
       <c r="U10" s="21"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>11</v>
       </c>
@@ -4998,7 +5000,7 @@
         <v>12321</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>12</v>
       </c>
@@ -5071,7 +5073,7 @@
         <v>16777</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>13</v>
       </c>
@@ -5144,7 +5146,7 @@
         <v>18135</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>14</v>
       </c>
@@ -5215,7 +5217,7 @@
       </c>
       <c r="U14" s="21"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
@@ -5288,7 +5290,7 @@
         <v>3124</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>16</v>
       </c>
@@ -5359,7 +5361,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>17</v>
       </c>
@@ -5432,7 +5434,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>18</v>
       </c>
@@ -5503,7 +5505,7 @@
       </c>
       <c r="U18" s="21"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -5574,7 +5576,7 @@
         <v>2836</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>20</v>
       </c>
@@ -5646,7 +5648,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>21</v>
       </c>
@@ -5717,7 +5719,7 @@
       </c>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>22</v>
       </c>
@@ -5790,7 +5792,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>23</v>
       </c>
@@ -5859,7 +5861,7 @@
       </c>
       <c r="U23" s="21"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>24</v>
       </c>
@@ -5929,7 +5931,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>25</v>
       </c>
@@ -6002,7 +6004,7 @@
         <v>5299</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
@@ -6071,7 +6073,7 @@
       </c>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>27</v>
       </c>
@@ -6144,7 +6146,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>28</v>
       </c>
@@ -6213,7 +6215,7 @@
       </c>
       <c r="U28" s="21"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>29</v>
       </c>
@@ -6286,7 +6288,7 @@
         <v>11079</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>30</v>
       </c>
@@ -6359,7 +6361,7 @@
         <v>3597</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
         <v>31</v>
       </c>
@@ -6429,7 +6431,7 @@
         <v>2551</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
         <v>32</v>
       </c>
@@ -6499,7 +6501,7 @@
         <v>2612</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
         <v>33</v>
       </c>
@@ -6568,7 +6570,7 @@
         <v>2564</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
         <v>34</v>
       </c>
@@ -6638,7 +6640,7 @@
         <v>2441</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>35</v>
       </c>
@@ -6709,7 +6711,7 @@
       </c>
       <c r="U35" s="21"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>36</v>
       </c>
@@ -6780,7 +6782,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>37</v>
       </c>
@@ -6849,7 +6851,7 @@
       </c>
       <c r="U37" s="21"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>38</v>
       </c>
@@ -6922,7 +6924,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
         <v>39</v>
       </c>
@@ -6992,7 +6994,7 @@
         <v>2551</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
         <v>40</v>
       </c>
@@ -7062,7 +7064,7 @@
       </c>
       <c r="U40" s="21"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
         <v>41</v>
       </c>
@@ -7135,7 +7137,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="45">
         <v>101</v>
       </c>
@@ -7208,7 +7210,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="45" t="s">
         <v>42</v>
       </c>
@@ -7281,7 +7283,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="45">
         <v>102</v>
       </c>
@@ -7352,7 +7354,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="45">
         <v>103</v>
       </c>
@@ -7421,7 +7423,7 @@
       </c>
       <c r="U45" s="21"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="45">
         <v>104</v>
       </c>
@@ -7490,7 +7492,7 @@
       </c>
       <c r="U46" s="21"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="45">
         <v>105</v>
       </c>
@@ -7561,7 +7563,7 @@
       </c>
       <c r="U47" s="21"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="45">
         <v>106</v>
       </c>
@@ -7632,7 +7634,7 @@
       </c>
       <c r="U48" s="21"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="45" t="s">
         <v>43</v>
       </c>
@@ -7701,7 +7703,7 @@
       </c>
       <c r="U49" s="21"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="45">
         <v>107</v>
       </c>
@@ -7774,7 +7776,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="45">
         <v>108</v>
       </c>
@@ -7843,7 +7845,7 @@
       </c>
       <c r="U51" s="21"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="45" t="s">
         <v>44</v>
       </c>
@@ -7914,7 +7916,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="45">
         <v>109</v>
       </c>
@@ -7987,7 +7989,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="45">
         <v>110</v>
       </c>
@@ -8056,7 +8058,7 @@
       </c>
       <c r="U54" s="21"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="45">
         <v>111</v>
       </c>
@@ -8129,7 +8131,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="45">
         <v>112</v>
       </c>
@@ -8198,7 +8200,7 @@
       </c>
       <c r="U56" s="21"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="45" t="s">
         <v>45</v>
       </c>
@@ -8269,7 +8271,7 @@
         <v>2707</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="45">
         <v>114</v>
       </c>
@@ -8337,7 +8339,7 @@
       </c>
       <c r="U58" s="21"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="45" t="s">
         <v>46</v>
       </c>
@@ -8410,7 +8412,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="45" t="s">
         <v>47</v>
       </c>
@@ -8483,7 +8485,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="45">
         <v>115</v>
       </c>
@@ -8552,7 +8554,7 @@
       </c>
       <c r="U61" s="21"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="45">
         <v>116</v>
       </c>
@@ -8621,7 +8623,7 @@
       </c>
       <c r="U62" s="21"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="45">
         <v>117</v>
       </c>
@@ -8690,7 +8692,7 @@
       </c>
       <c r="U63" s="21"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="45">
         <v>118</v>
       </c>
@@ -8763,7 +8765,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="45">
         <v>119</v>
       </c>
@@ -8834,7 +8836,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="45">
         <v>120</v>
       </c>
@@ -8903,7 +8905,7 @@
       </c>
       <c r="U66" s="21"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="45">
         <v>121</v>
       </c>
@@ -8974,7 +8976,7 @@
       </c>
       <c r="U67" s="21"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="45" t="s">
         <v>158</v>
       </c>
@@ -9045,7 +9047,7 @@
       </c>
       <c r="U68" s="21"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="45">
         <v>123</v>
       </c>
@@ -9116,7 +9118,7 @@
       </c>
       <c r="U69" s="21"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="45">
         <v>124</v>
       </c>
@@ -9185,9 +9187,11 @@
         <f t="shared" si="29"/>
         <v>848</v>
       </c>
-      <c r="U70" s="21"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U70" s="21">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" s="45">
         <v>125</v>
       </c>
@@ -9258,7 +9262,7 @@
       </c>
       <c r="U71" s="21"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="45">
         <v>126</v>
       </c>
@@ -9328,7 +9332,7 @@
         <v>2736</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="21"/>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -9370,10 +9374,10 @@
       <c r="T73" s="21"/>
       <c r="U73" s="20">
         <f>SUM(U2:U72)</f>
-        <v>132338</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>133186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="21"/>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -9405,7 +9409,7 @@
       <c r="T74" s="21"/>
       <c r="U74" s="21"/>
     </row>
-    <row r="75" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
@@ -9448,20 +9452,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C901BC-37D1-4CF5-9271-04B7C9971E6A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
     <col min="3" max="3" width="25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>197</v>
       </c>
@@ -9478,13 +9482,13 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>209</v>
       </c>
       <c r="C2" s="3">
         <f>'Maintenance_01-Apr-2025_Onwards'!K74</f>
-        <v>286205</v>
+        <v>288834</v>
       </c>
       <c r="D2" s="62">
         <v>45686</v>
@@ -9499,13 +9503,13 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>210</v>
       </c>
       <c r="C3" s="3">
         <f>EB!U73</f>
-        <v>132338</v>
+        <v>133186</v>
       </c>
       <c r="D3" s="62">
         <v>45706</v>
@@ -9520,7 +9524,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D4" s="62">
         <v>45733</v>
       </c>
@@ -9534,7 +9538,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D5" s="62">
         <v>45727</v>
       </c>
@@ -9548,7 +9552,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D6" s="62">
         <v>111491</v>
       </c>
@@ -9562,13 +9566,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>196</v>
       </c>
       <c r="C7" s="3">
         <f>SUM(C1:C6)</f>
-        <v>1060961</v>
+        <v>1064438</v>
       </c>
       <c r="D7" s="62">
         <v>45757</v>
@@ -9584,7 +9588,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D8" s="62">
         <v>45761</v>
       </c>
@@ -9598,7 +9602,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>186</v>
       </c>
@@ -9619,7 +9623,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>174</v>
       </c>
@@ -9640,13 +9644,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>175</v>
       </c>
       <c r="C11" s="3">
-        <f>17668+2566</f>
-        <v>20234</v>
+        <f>17668+2566+3477</f>
+        <v>23711</v>
       </c>
       <c r="D11" s="62">
         <v>45763</v>
@@ -9661,7 +9665,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>179</v>
       </c>
@@ -9682,7 +9686,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>211</v>
       </c>
@@ -9703,16 +9707,16 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>171913</v>
+        <v>175390</v>
       </c>
       <c r="E15" t="s">
         <v>172</v>
@@ -9722,28 +9726,28 @@
         <v>889456</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>202</v>
       </c>
       <c r="C17" s="3">
         <f>C7-F15</f>
-        <v>171505</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>174982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="38"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="48"/>
       <c r="B20" s="3" t="s">
         <v>203</v>
@@ -9754,15 +9758,15 @@
       </c>
       <c r="E20" s="38"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="48"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="48"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="11"/>
     </row>
   </sheetData>
@@ -9780,24 +9784,24 @@
       <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="8" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="11" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="12" max="13" width="8.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" customWidth="1"/>
-    <col min="15" max="15" width="36.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="12" max="13" width="8.88671875" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" customWidth="1"/>
+    <col min="15" max="15" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -9845,7 +9849,7 @@
       </c>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -9896,7 +9900,7 @@
       <c r="O2" s="21"/>
       <c r="P2" s="17"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -9945,7 +9949,7 @@
       <c r="O3" s="21"/>
       <c r="P3" s="17"/>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -9992,7 +9996,7 @@
       <c r="O4" s="21"/>
       <c r="P4" s="8"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -10041,7 +10045,7 @@
       <c r="O5" s="21"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -10092,7 +10096,7 @@
       <c r="O6" s="21"/>
       <c r="P6" s="17"/>
     </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -10141,7 +10145,7 @@
       <c r="O7" s="21"/>
       <c r="P7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -10188,7 +10192,7 @@
       <c r="O8" s="21"/>
       <c r="P8" s="8"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -10235,7 +10239,7 @@
       <c r="O9" s="21"/>
       <c r="P9" s="8"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -10280,7 +10284,7 @@
       <c r="O10" s="21"/>
       <c r="P10" s="8"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -10329,7 +10333,7 @@
       <c r="O11" s="21"/>
       <c r="P11" s="17"/>
     </row>
-    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -10380,7 +10384,7 @@
       <c r="O12" s="21"/>
       <c r="P12" s="17"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -10431,7 +10435,7 @@
       <c r="O13" s="21"/>
       <c r="P13" s="17"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -10482,7 +10486,7 @@
       <c r="O14" s="22"/>
       <c r="P14" s="8"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -10533,7 +10537,7 @@
       <c r="O15" s="21"/>
       <c r="P15" s="17"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -10584,7 +10588,7 @@
       <c r="O16" s="21"/>
       <c r="P16" s="17"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -10635,7 +10639,7 @@
       <c r="O17" s="21"/>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -10686,7 +10690,7 @@
       <c r="O18" s="21"/>
       <c r="P18" s="17"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -10733,7 +10737,7 @@
       <c r="O19" s="21"/>
       <c r="P19" s="8"/>
     </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -10784,7 +10788,7 @@
       <c r="O20" s="21"/>
       <c r="P20" s="17"/>
     </row>
-    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -10835,7 +10839,7 @@
       <c r="O21" s="21"/>
       <c r="P21" s="17"/>
     </row>
-    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -10886,7 +10890,7 @@
       <c r="O22" s="21"/>
       <c r="P22" s="17"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -10935,7 +10939,7 @@
       </c>
       <c r="P23" s="8"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -10982,7 +10986,7 @@
       <c r="O24" s="21"/>
       <c r="P24" s="8"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -11033,7 +11037,7 @@
       <c r="O25" s="21"/>
       <c r="P25" s="17"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -11080,7 +11084,7 @@
       <c r="O26" s="21"/>
       <c r="P26" s="8"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -11131,7 +11135,7 @@
       <c r="O27" s="21"/>
       <c r="P27" s="17"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -11178,7 +11182,7 @@
       <c r="O28" s="21"/>
       <c r="P28" s="8"/>
     </row>
-    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -11225,7 +11229,7 @@
       <c r="O29" s="21"/>
       <c r="P29" s="8"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -11274,7 +11278,7 @@
       <c r="O30" s="21"/>
       <c r="P30" s="17"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -11325,7 +11329,7 @@
       <c r="O31" s="21"/>
       <c r="P31" s="17"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -11374,7 +11378,7 @@
       <c r="O32" s="21"/>
       <c r="P32" s="17"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -11423,7 +11427,7 @@
       <c r="O33" s="21"/>
       <c r="P33" s="17"/>
     </row>
-    <row r="34" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -11470,7 +11474,7 @@
       <c r="O34" s="21"/>
       <c r="P34" s="8"/>
     </row>
-    <row r="35" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -11519,7 +11523,7 @@
       <c r="O35" s="21"/>
       <c r="P35" s="8"/>
     </row>
-    <row r="36" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -11566,7 +11570,7 @@
       <c r="O36" s="22"/>
       <c r="P36" s="8"/>
     </row>
-    <row r="37" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -11615,7 +11619,7 @@
       <c r="O37" s="21"/>
       <c r="P37" s="8"/>
     </row>
-    <row r="38" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -11666,7 +11670,7 @@
       <c r="O38" s="21"/>
       <c r="P38" s="8"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -11713,7 +11717,7 @@
       <c r="O39" s="21"/>
       <c r="P39" s="8"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -11764,7 +11768,7 @@
       <c r="O40" s="21"/>
       <c r="P40" s="17"/>
     </row>
-    <row r="41" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -11815,7 +11819,7 @@
       <c r="O41" s="21"/>
       <c r="P41" s="17"/>
     </row>
-    <row r="42" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -11868,7 +11872,7 @@
       </c>
       <c r="P42" s="17"/>
     </row>
-    <row r="43" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -11921,7 +11925,7 @@
       </c>
       <c r="P43" s="17"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -11968,7 +11972,7 @@
       <c r="O44" s="21"/>
       <c r="P44" s="8"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -12017,7 +12021,7 @@
       <c r="O45" s="21"/>
       <c r="P45" s="8"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -12066,7 +12070,7 @@
       <c r="O46" s="21"/>
       <c r="P46" s="8"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -12118,7 +12122,7 @@
       <c r="R47" s="19"/>
       <c r="S47" s="19"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -12169,7 +12173,7 @@
       <c r="O48" s="22"/>
       <c r="P48" s="17"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -12216,7 +12220,7 @@
       <c r="O49" s="21"/>
       <c r="P49" s="8"/>
     </row>
-    <row r="50" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -12267,7 +12271,7 @@
       <c r="O50" s="21"/>
       <c r="P50" s="17"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -12316,7 +12320,7 @@
       <c r="O51" s="21"/>
       <c r="P51" s="17"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -12365,7 +12369,7 @@
       <c r="O52" s="21"/>
       <c r="P52" s="17"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -12416,7 +12420,7 @@
       <c r="O53" s="21"/>
       <c r="P53" s="8"/>
     </row>
-    <row r="54" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -12465,7 +12469,7 @@
       <c r="O54" s="22"/>
       <c r="P54" s="8"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -12515,7 +12519,7 @@
       <c r="O55" s="22"/>
       <c r="P55" s="8"/>
     </row>
-    <row r="56" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -12564,7 +12568,7 @@
       <c r="O56" s="22"/>
       <c r="P56" s="8"/>
     </row>
-    <row r="57" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -12611,7 +12615,7 @@
       <c r="O57" s="22"/>
       <c r="P57" s="8"/>
     </row>
-    <row r="58" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -12660,7 +12664,7 @@
       </c>
       <c r="P58" s="8"/>
     </row>
-    <row r="59" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -12709,7 +12713,7 @@
       <c r="O59" s="21"/>
       <c r="P59" s="17"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -12758,7 +12762,7 @@
       <c r="O60" s="21"/>
       <c r="P60" s="8"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -12805,7 +12809,7 @@
       <c r="O61" s="21"/>
       <c r="P61" s="8"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -12852,7 +12856,7 @@
       <c r="O62" s="21"/>
       <c r="P62" s="8"/>
     </row>
-    <row r="63" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -12899,7 +12903,7 @@
       <c r="O63" s="21"/>
       <c r="P63" s="8"/>
     </row>
-    <row r="64" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -12950,7 +12954,7 @@
       <c r="O64" s="21"/>
       <c r="P64" s="17"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -12997,7 +13001,7 @@
       <c r="O65" s="21"/>
       <c r="P65" s="8"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -13044,7 +13048,7 @@
       <c r="O66" s="21"/>
       <c r="P66" s="8"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -13093,7 +13097,7 @@
       <c r="O67" s="21"/>
       <c r="P67" s="8"/>
     </row>
-    <row r="68" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -13144,7 +13148,7 @@
       <c r="O68" s="22"/>
       <c r="P68" s="8"/>
     </row>
-    <row r="69" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -13193,7 +13197,7 @@
       <c r="O69" s="22"/>
       <c r="P69" s="8"/>
     </row>
-    <row r="70" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -13244,7 +13248,7 @@
       <c r="O70" s="22"/>
       <c r="P70" s="8"/>
     </row>
-    <row r="71" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -13295,7 +13299,7 @@
       <c r="O71" s="21"/>
       <c r="P71" s="17"/>
     </row>
-    <row r="72" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -13344,7 +13348,7 @@
       <c r="O72" s="21"/>
       <c r="P72" s="8"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -13391,7 +13395,7 @@
       <c r="O73" s="21"/>
       <c r="P73" s="8"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E74" s="3">
         <f>SUM(E2:E73)</f>
         <v>57993</v>
@@ -13421,7 +13425,7 @@
       </c>
       <c r="N74" s="19"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D77" t="s">
         <v>163</v>
       </c>
@@ -13430,7 +13434,7 @@
         <v>719150</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D78" s="2" t="s">
         <v>164</v>
       </c>
@@ -13439,28 +13443,28 @@
         <v>430473</v>
       </c>
     </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D84"/>
       <c r="E84"/>
       <c r="F84" s="42"/>
       <c r="H84" s="23"/>
       <c r="I84" s="19"/>
     </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D85"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D86" s="38"/>
       <c r="E86"/>
       <c r="F86" s="42"/>
       <c r="H86" s="38"/>
     </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D87"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D88"/>
       <c r="E88"/>
     </row>
@@ -13479,15 +13483,15 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
     <col min="3" max="3" width="25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>165</v>
       </c>
@@ -13503,7 +13507,7 @@
         <v>312867.11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>161</v>
       </c>
@@ -13519,7 +13523,7 @@
         <v>211945</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>166</v>
       </c>
@@ -13535,7 +13539,7 @@
         <v>100922.10999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>168</v>
       </c>
@@ -13544,12 +13548,12 @@
         <v>642418</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>176</v>
       </c>
@@ -13557,7 +13561,7 @@
         <v>18043</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>170</v>
       </c>
@@ -13568,7 +13572,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="48">
         <v>45733</v>
       </c>
@@ -13582,7 +13586,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="48">
         <v>45727</v>
       </c>
@@ -13593,7 +13597,7 @@
         <v>29811</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="48">
         <v>45748</v>
       </c>
@@ -13604,7 +13608,7 @@
         <v>3630</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>172</v>
       </c>
@@ -13613,7 +13617,7 @@
         <v>416100</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>173</v>
       </c>
@@ -13622,7 +13626,7 @@
         <v>226318</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>186</v>
       </c>
@@ -13630,7 +13634,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>174</v>
       </c>
@@ -13639,7 +13643,7 @@
         <v>117636</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>175</v>
       </c>
@@ -13648,7 +13652,7 @@
         <v>67347</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>179</v>
       </c>
@@ -13657,7 +13661,7 @@
         <v>40543</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>146</v>
       </c>
@@ -13666,7 +13670,7 @@
         <v>226896</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>180</v>
       </c>
@@ -13688,18 +13692,18 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="11"/>
-    <col min="3" max="3" width="10.7109375" style="11" customWidth="1"/>
-    <col min="4" max="5" width="12.140625" style="11" customWidth="1"/>
-    <col min="6" max="7" width="13.85546875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="11"/>
+    <col min="3" max="3" width="10.6640625" style="11" customWidth="1"/>
+    <col min="4" max="5" width="12.109375" style="11" customWidth="1"/>
+    <col min="6" max="7" width="13.88671875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>212</v>
       </c>
@@ -13720,7 +13724,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="68" t="s">
         <v>218</v>
       </c>
@@ -13743,7 +13747,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>215</v>
       </c>
@@ -13763,7 +13767,7 @@
         <v>3548</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>111</v>
       </c>
@@ -13783,7 +13787,7 @@
         <v>7086</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>216</v>
       </c>
@@ -13803,7 +13807,7 @@
         <v>22063</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>39</v>
       </c>
@@ -13823,7 +13827,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
@@ -13843,7 +13847,7 @@
         <v>24798</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>45</v>
       </c>
@@ -13863,7 +13867,7 @@
         <v>4006</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>217</v>
       </c>
@@ -13883,7 +13887,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>126</v>
       </c>
@@ -13903,7 +13907,7 @@
         <v>14384</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
@@ -13923,7 +13927,7 @@
         <v>4016</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>219</v>
       </c>
@@ -13937,7 +13941,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
@@ -13951,7 +13955,7 @@
         <v>21772</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>222</v>
       </c>
@@ -13965,7 +13969,7 @@
         <v>3430</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C17" s="11" t="s">
         <v>47</v>
       </c>
@@ -13974,7 +13978,7 @@
         <v>4397</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C18" s="11" t="s">
         <v>5</v>
       </c>
@@ -13982,17 +13986,17 @@
         <v>11114</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D19" s="11">
         <v>53000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
105 and g11 payments updated
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30426273-72ED-403C-9D0F-69810250C4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BB22FB-CFF4-4D92-B670-4BFE48E77739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance_01-Apr-2025_Onwards" sheetId="9" r:id="rId1"/>
@@ -980,7 +980,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1164,17 +1164,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1523,7 +1512,7 @@
     <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,7 +1746,9 @@
         <f t="shared" si="0"/>
         <v>2774</v>
       </c>
-      <c r="K6" s="21"/>
+      <c r="K6" s="21">
+        <v>2774</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -2041,7 +2032,9 @@
         <f t="shared" si="0"/>
         <v>2456</v>
       </c>
-      <c r="K14" s="21"/>
+      <c r="K14" s="21">
+        <v>2456</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -2339,7 +2332,7 @@
         <v>3146</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2355,10 +2348,10 @@
       <c r="E23" s="26">
         <v>788</v>
       </c>
-      <c r="F23" s="71">
+      <c r="F23" s="50">
         <v>4.54</v>
       </c>
-      <c r="G23" s="70">
+      <c r="G23" s="15">
         <f t="shared" si="1"/>
         <v>3578</v>
       </c>
@@ -2372,7 +2365,7 @@
         <f t="shared" si="0"/>
         <v>13427</v>
       </c>
-      <c r="K23" s="72"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
@@ -2810,14 +2803,14 @@
       </c>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:13" s="73" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="74" t="s">
+      <c r="C36" s="69" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="26">
@@ -2826,10 +2819,10 @@
       <c r="E36" s="26">
         <v>872</v>
       </c>
-      <c r="F36" s="71">
+      <c r="F36" s="50">
         <v>4.54</v>
       </c>
-      <c r="G36" s="70">
+      <c r="G36" s="15">
         <f t="shared" si="1"/>
         <v>3959</v>
       </c>
@@ -2843,7 +2836,7 @@
         <f t="shared" si="0"/>
         <v>14858</v>
       </c>
-      <c r="K36" s="72">
+      <c r="K36" s="21">
         <v>14858</v>
       </c>
     </row>
@@ -3244,7 +3237,9 @@
         <f t="shared" si="0"/>
         <v>3187</v>
       </c>
-      <c r="K47" s="20"/>
+      <c r="K47" s="20">
+        <v>3187</v>
+      </c>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
     </row>
@@ -3634,7 +3629,7 @@
       <c r="H58" s="26">
         <v>9813</v>
       </c>
-      <c r="I58" s="75">
+      <c r="I58" s="70">
         <v>3564</v>
       </c>
       <c r="J58" s="26">
@@ -4009,20 +4004,20 @@
       <c r="A69" s="6">
         <v>68</v>
       </c>
-      <c r="B69" s="69" t="s">
+      <c r="B69" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C69" s="68" t="s">
         <v>235</v>
       </c>
       <c r="D69" s="34"/>
-      <c r="E69" s="70">
+      <c r="E69" s="15">
         <v>802</v>
       </c>
       <c r="F69" s="50">
         <v>4.54</v>
       </c>
-      <c r="G69" s="70">
+      <c r="G69" s="15">
         <f t="shared" si="3"/>
         <v>3641</v>
       </c>
@@ -4197,7 +4192,7 @@
       </c>
       <c r="K74">
         <f>SUM(K2:K73)</f>
-        <v>295223</v>
+        <v>303640</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -4240,8 +4235,8 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N47" sqref="N47"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5234,7 +5229,9 @@
         <f t="shared" si="8"/>
         <v>7799</v>
       </c>
-      <c r="U14" s="21"/>
+      <c r="U14" s="21">
+        <v>7799</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
@@ -9395,7 +9392,7 @@
       <c r="T73" s="21"/>
       <c r="U73" s="20">
         <f>SUM(U2:U72)</f>
-        <v>140912</v>
+        <v>148711</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -9473,7 +9470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C901BC-37D1-4CF5-9271-04B7C9971E6A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="134" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -9509,7 +9506,7 @@
       </c>
       <c r="C2" s="3">
         <f>'Maintenance_01-Apr-2025_Onwards'!K74</f>
-        <v>295223</v>
+        <v>303640</v>
       </c>
       <c r="D2" s="61">
         <v>45686</v>
@@ -9530,7 +9527,7 @@
       </c>
       <c r="C3" s="3">
         <f>EB!U73</f>
-        <v>140912</v>
+        <v>148711</v>
       </c>
       <c r="D3" s="61">
         <v>45706</v>
@@ -9593,7 +9590,7 @@
       </c>
       <c r="C7" s="3">
         <f>SUM(C1:C6)</f>
-        <v>1078553</v>
+        <v>1094769</v>
       </c>
       <c r="D7" s="61">
         <v>45757</v>
@@ -9649,8 +9646,8 @@
         <v>174</v>
       </c>
       <c r="C10" s="3">
-        <f>91651+6687-10000+2700-36400-10000</f>
-        <v>44638</v>
+        <f>91651+6687-10000+2700-36400-10000+2774</f>
+        <v>47412</v>
       </c>
       <c r="D10" s="61">
         <v>45761</v>
@@ -9670,8 +9667,8 @@
         <v>175</v>
       </c>
       <c r="C11" s="3">
-        <f>17668+2566+3477+7726+6389</f>
-        <v>37826</v>
+        <f>17668+2566+3477+7726+6389+3187+10255</f>
+        <v>51268</v>
       </c>
       <c r="D11" s="61">
         <v>45763</v>
@@ -9749,7 +9746,7 @@
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>179505</v>
+        <v>195721</v>
       </c>
       <c r="E15" t="s">
         <v>172</v>
@@ -9768,7 +9765,7 @@
       </c>
       <c r="C17" s="3">
         <f>C7-F15</f>
-        <v>179097</v>
+        <v>195313</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
120 m and e paid
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BB22FB-CFF4-4D92-B670-4BFE48E77739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A274FF1C-4BAC-42CF-9E43-047BFEBC5810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance_01-Apr-2025_Onwards" sheetId="9" r:id="rId1"/>
@@ -1509,10 +1509,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E3C748-2165-4E26-87D0-2D40C997FFD8}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3926,7 +3926,9 @@
         <f t="shared" si="0"/>
         <v>11893</v>
       </c>
-      <c r="K66" s="21"/>
+      <c r="K66" s="21">
+        <v>11893</v>
+      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
@@ -4192,7 +4194,7 @@
       </c>
       <c r="K74">
         <f>SUM(K2:K73)</f>
-        <v>303640</v>
+        <v>315533</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -4236,7 +4238,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V14" sqref="V14"/>
+      <selection pane="bottomLeft" activeCell="V66" sqref="V66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8921,7 +8923,9 @@
         <f t="shared" ref="T66:T72" si="29">ROUND(O66+S66,0)</f>
         <v>2634</v>
       </c>
-      <c r="U66" s="21"/>
+      <c r="U66" s="21">
+        <v>2634</v>
+      </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="45">
@@ -9392,7 +9396,7 @@
       <c r="T73" s="21"/>
       <c r="U73" s="20">
         <f>SUM(U2:U72)</f>
-        <v>148711</v>
+        <v>151345</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -9470,8 +9474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C901BC-37D1-4CF5-9271-04B7C9971E6A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9506,7 +9510,7 @@
       </c>
       <c r="C2" s="3">
         <f>'Maintenance_01-Apr-2025_Onwards'!K74</f>
-        <v>303640</v>
+        <v>315533</v>
       </c>
       <c r="D2" s="61">
         <v>45686</v>
@@ -9527,7 +9531,7 @@
       </c>
       <c r="C3" s="3">
         <f>EB!U73</f>
-        <v>148711</v>
+        <v>151345</v>
       </c>
       <c r="D3" s="61">
         <v>45706</v>
@@ -9590,7 +9594,7 @@
       </c>
       <c r="C7" s="3">
         <f>SUM(C1:C6)</f>
-        <v>1094769</v>
+        <v>1109296</v>
       </c>
       <c r="D7" s="61">
         <v>45757</v>
@@ -9688,8 +9692,8 @@
         <v>179</v>
       </c>
       <c r="C12" s="3">
-        <f>92538+4215</f>
-        <v>96753</v>
+        <f>92538+4215+14527</f>
+        <v>111280</v>
       </c>
       <c r="D12" s="61">
         <v>45756</v>
@@ -9746,7 +9750,7 @@
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>195721</v>
+        <v>210248</v>
       </c>
       <c r="E15" t="s">
         <v>172</v>
@@ -9765,7 +9769,7 @@
       </c>
       <c r="C17" s="3">
         <f>C7-F15</f>
-        <v>195313</v>
+        <v>209840</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
g05 m and e paid
</commit_message>
<xml_diff>
--- a/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
+++ b/Maintenance_Sheet_01-Apr-2025_Onwards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theho\Desktop\oxygengit\maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A274FF1C-4BAC-42CF-9E43-047BFEBC5810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15321823-70EF-4FC8-BAF5-8223D823A6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18F95FEC-B9AA-4F82-AECF-118895130A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance_01-Apr-2025_Onwards" sheetId="9" r:id="rId1"/>
@@ -1509,10 +1509,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E3C748-2165-4E26-87D0-2D40C997FFD8}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="134" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4237,8 +4237,8 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V66" sqref="V66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4665,7 +4665,9 @@
         <f t="shared" si="8"/>
         <v>10203</v>
       </c>
-      <c r="U6" s="21"/>
+      <c r="U6" s="21">
+        <v>10203</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -9396,7 +9398,7 @@
       <c r="T73" s="21"/>
       <c r="U73" s="20">
         <f>SUM(U2:U72)</f>
-        <v>151345</v>
+        <v>161548</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -9474,8 +9476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C901BC-37D1-4CF5-9271-04B7C9971E6A}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9531,7 +9533,7 @@
       </c>
       <c r="C3" s="3">
         <f>EB!U73</f>
-        <v>151345</v>
+        <v>161548</v>
       </c>
       <c r="D3" s="61">
         <v>45706</v>
@@ -9594,7 +9596,7 @@
       </c>
       <c r="C7" s="3">
         <f>SUM(C1:C6)</f>
-        <v>1109296</v>
+        <v>1119499</v>
       </c>
       <c r="D7" s="61">
         <v>45757</v>
@@ -9650,8 +9652,8 @@
         <v>174</v>
       </c>
       <c r="C10" s="3">
-        <f>91651+6687-10000+2700-36400-10000+2774</f>
-        <v>47412</v>
+        <f>91651+6687-10000+2700-36400-10000+2774+10203</f>
+        <v>57615</v>
       </c>
       <c r="D10" s="61">
         <v>45761</v>
@@ -9750,7 +9752,7 @@
       </c>
       <c r="C15" s="3">
         <f>SUM(C9:C14)</f>
-        <v>210248</v>
+        <v>220451</v>
       </c>
       <c r="E15" t="s">
         <v>172</v>
@@ -9769,7 +9771,7 @@
       </c>
       <c r="C17" s="3">
         <f>C7-F15</f>
-        <v>209840</v>
+        <v>220043</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>